<commit_message>
scrapes more attributes and skips players with insufficient data
read_through_names.py now collects weight, height
also skips players who have played fewer than 5 games
</commit_message>
<xml_diff>
--- a/2017_data/Andy_Dalton_QB_2017.xlsx
+++ b/2017_data/Andy_Dalton_QB_2017.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -394,6 +394,16 @@
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
+          <t>height</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>weight</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
           <t>fantasy points</t>
         </is>
       </c>
@@ -418,6 +428,12 @@
         <v>0</v>
       </c>
       <c r="G2" t="n">
+        <v>6.166666666666667</v>
+      </c>
+      <c r="H2" t="n">
+        <v>220</v>
+      </c>
+      <c r="I2" t="n">
         <v>-3</v>
       </c>
     </row>
@@ -441,6 +457,12 @@
         <v>0</v>
       </c>
       <c r="G3" t="n">
+        <v>6.166666666666667</v>
+      </c>
+      <c r="H3" t="n">
+        <v>220</v>
+      </c>
+      <c r="I3" t="n">
         <v>9.460000000000001</v>
       </c>
     </row>
@@ -464,6 +486,12 @@
         <v>0</v>
       </c>
       <c r="G4" t="n">
+        <v>6.166666666666667</v>
+      </c>
+      <c r="H4" t="n">
+        <v>220</v>
+      </c>
+      <c r="I4" t="n">
         <v>16.28</v>
       </c>
     </row>
@@ -487,6 +515,12 @@
         <v>0</v>
       </c>
       <c r="G5" t="n">
+        <v>6.166666666666667</v>
+      </c>
+      <c r="H5" t="n">
+        <v>220</v>
+      </c>
+      <c r="I5" t="n">
         <v>28.34</v>
       </c>
     </row>
@@ -510,6 +544,12 @@
         <v>0</v>
       </c>
       <c r="G6" t="n">
+        <v>6.166666666666667</v>
+      </c>
+      <c r="H6" t="n">
+        <v>220</v>
+      </c>
+      <c r="I6" t="n">
         <v>13.32</v>
       </c>
     </row>
@@ -533,6 +573,12 @@
         <v>0</v>
       </c>
       <c r="G7" t="n">
+        <v>6.166666666666667</v>
+      </c>
+      <c r="H7" t="n">
+        <v>220</v>
+      </c>
+      <c r="I7" t="n">
         <v>10.4</v>
       </c>
     </row>
@@ -556,6 +602,12 @@
         <v>0</v>
       </c>
       <c r="G8" t="n">
+        <v>6.166666666666667</v>
+      </c>
+      <c r="H8" t="n">
+        <v>220</v>
+      </c>
+      <c r="I8" t="n">
         <v>18.72</v>
       </c>
     </row>
@@ -579,6 +631,12 @@
         <v>0</v>
       </c>
       <c r="G9" t="n">
+        <v>6.166666666666667</v>
+      </c>
+      <c r="H9" t="n">
+        <v>220</v>
+      </c>
+      <c r="I9" t="n">
         <v>5.34</v>
       </c>
     </row>
@@ -602,6 +660,12 @@
         <v>0</v>
       </c>
       <c r="G10" t="n">
+        <v>6.166666666666667</v>
+      </c>
+      <c r="H10" t="n">
+        <v>220</v>
+      </c>
+      <c r="I10" t="n">
         <v>14.6</v>
       </c>
     </row>
@@ -625,6 +689,12 @@
         <v>0</v>
       </c>
       <c r="G11" t="n">
+        <v>6.166666666666667</v>
+      </c>
+      <c r="H11" t="n">
+        <v>220</v>
+      </c>
+      <c r="I11" t="n">
         <v>18.56</v>
       </c>
     </row>
@@ -648,6 +718,12 @@
         <v>0</v>
       </c>
       <c r="G12" t="n">
+        <v>6.166666666666667</v>
+      </c>
+      <c r="H12" t="n">
+        <v>220</v>
+      </c>
+      <c r="I12" t="n">
         <v>19.16</v>
       </c>
     </row>
@@ -671,6 +747,12 @@
         <v>0</v>
       </c>
       <c r="G13" t="n">
+        <v>6.166666666666667</v>
+      </c>
+      <c r="H13" t="n">
+        <v>220</v>
+      </c>
+      <c r="I13" t="n">
         <v>19.26</v>
       </c>
     </row>
@@ -694,6 +776,12 @@
         <v>0</v>
       </c>
       <c r="G14" t="n">
+        <v>6.166666666666667</v>
+      </c>
+      <c r="H14" t="n">
+        <v>220</v>
+      </c>
+      <c r="I14" t="n">
         <v>7.64</v>
       </c>
     </row>
@@ -717,6 +805,12 @@
         <v>0</v>
       </c>
       <c r="G15" t="n">
+        <v>6.166666666666667</v>
+      </c>
+      <c r="H15" t="n">
+        <v>220</v>
+      </c>
+      <c r="I15" t="n">
         <v>0.52</v>
       </c>
     </row>
@@ -740,6 +834,12 @@
         <v>0</v>
       </c>
       <c r="G16" t="n">
+        <v>6.166666666666667</v>
+      </c>
+      <c r="H16" t="n">
+        <v>220</v>
+      </c>
+      <c r="I16" t="n">
         <v>11.42</v>
       </c>
     </row>
@@ -763,6 +863,12 @@
         <v>0</v>
       </c>
       <c r="G17" t="n">
+        <v>6.166666666666667</v>
+      </c>
+      <c r="H17" t="n">
+        <v>220</v>
+      </c>
+      <c r="I17" t="n">
         <v>20.68</v>
       </c>
     </row>

</xml_diff>